<commit_message>
adicionado ata de hoje e avançõs na tabela de riscos
</commit_message>
<xml_diff>
--- a/Documentação/Gestão/Gestão de riscos .xlsx
+++ b/Documentação/Gestão/Gestão de riscos .xlsx
@@ -1,19 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fb330565894022c/Área de Trabalho/Strawtech/Sprint2/Sprint2/Documentação/Gestão/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="52" documentId="11_CF4C787892D7E5F60EE01957CA2528E350C20E1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1E22D98-0368-475C-A6EC-52FE56E0582A}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Página1'!$B$2:$H$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Página1!$B$2:$H$9</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -54,9 +77,6 @@
     <t>Criação de um token para cada fazenda do usuário</t>
   </si>
   <si>
-    <t>Desfalque de um membro do grupo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dificuldade de comunicação entre integrantes da
 equipe
 </t>
@@ -72,26 +92,51 @@
   </si>
   <si>
     <t>Instalação realizada visando os possíveis danos aos componentes utilizados (sensores, fios, etc)</t>
+  </si>
+  <si>
+    <t>Desfalque de algum membro do grupo</t>
+  </si>
+  <si>
+    <t>Projeto desorganizado</t>
+  </si>
+  <si>
+    <t>Projeto dividido e organizado nas ferramentas de gestão ,juntamente com daily's</t>
+  </si>
+  <si>
+    <t>Manter os integrantes engajados com o projeto</t>
+  </si>
+  <si>
+    <t>Aumentar o fluxo de comunicação entre o grupo e flexibilização nos horários das daily's para evitar ausências</t>
+  </si>
+  <si>
+    <t>Ter a disponibilidade de frequentar diversos pontos de conexão a rede</t>
+  </si>
+  <si>
+    <t>Sprints desbalanceadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazendo as estimatívas dos tamanhos dos requisitos e criando o gráfico de Burndown </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -102,7 +147,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -129,21 +174,13 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
-    <border/>
+  <borders count="9">
     <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -155,17 +192,36 @@
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -180,8 +236,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
@@ -191,6 +249,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -199,113 +258,140 @@
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF00FF00"/>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FF434343"/>
+          <bgColor rgb="FF434343"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF434343"/>
-          <bgColor rgb="FF434343"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -495,24 +581,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="7" width="17.63"/>
-    <col customWidth="1" min="8" max="8" width="31.0"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -529,7 +625,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -560,22 +656,22 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" ht="52.5" customHeight="1">
+    <row r="3" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" ref="F3:F9" si="1">PRODUCT(D3:E3)</f>
+        <f t="shared" ref="F3:F9" si="0">PRODUCT(D3:E3)</f>
         <v>3</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -592,28 +688,30 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" ht="52.5" customHeight="1">
+    <row r="4" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -622,26 +720,30 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" ht="52.5" customHeight="1">
+    <row r="5" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="F5" s="9">
-        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -650,28 +752,30 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" ht="52.5" customHeight="1">
+    <row r="6" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="F6" s="7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -680,29 +784,29 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" ht="52.5" customHeight="1">
+    <row r="7" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="6">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="1"/>
@@ -712,20 +816,30 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" ht="52.5" customHeight="1">
+    <row r="8" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="7">
-        <v>6.0</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
       <c r="F8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -734,20 +848,30 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" ht="52.5" customHeight="1">
+    <row r="9" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="B9" s="10">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="10">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10">
+        <v>3</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -756,16 +880,18 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="1"/>
+    <row r="10" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="11">
+        <v>8</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -773,16 +899,18 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+    <row r="11" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -793,15 +921,15 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -813,7 +941,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -833,7 +961,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -853,7 +981,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -873,7 +1001,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -892,7 +1020,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -911,7 +1039,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -931,7 +1059,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -951,7 +1079,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -971,7 +1099,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -991,7 +1119,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1010,7 +1138,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1029,7 +1157,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1047,7 +1175,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1065,7 +1193,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1083,7 +1211,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1100,39 +1228,33 @@
       <c r="N27" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="$B$2:$H$9"/>
-  <conditionalFormatting sqref="F3:F10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>1</formula>
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F10">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>3</formula>
-      <formula>4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3 F4 F5 F6 F7 F8 F9">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <autoFilter ref="B2:H9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="F3:F9">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>9</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="notContainsText" dxfId="3" priority="5" operator="notContains" text="1, 2, 3, 4, 6, 9">
-      <formula>ISERROR(SEARCH(("1, 2, 3, 4, 6, 9"),(F5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3 F4 F5 F6 F7 F8 F9">
     <cfRule type="notContainsText" dxfId="4" priority="6" operator="notContains" text="1, 2, 3, 4, 6, 9">
       <formula>ISERROR(SEARCH(("1, 2, 3, 4, 6, 9"),(F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <conditionalFormatting sqref="F3:F10">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+      <formula>1</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="notContainsText" dxfId="0" priority="5" operator="notContains" text="1, 2, 3, 4, 6, 9">
+      <formula>ISERROR(SEARCH(("1, 2, 3, 4, 6, 9"),(F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajusti Insert Erro e Validação insirida no site
</commit_message>
<xml_diff>
--- a/Documentação/Gestão/Gestão de riscos .xlsx
+++ b/Documentação/Gestão/Gestão de riscos .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fb330565894022c/Área de Trabalho/Strawtech/Sprint2/Sprint2/Documentação/Gestão/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_CF4C787892D7E5F60EE01957CA2528E350C20E1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1E22D98-0368-475C-A6EC-52FE56E0582A}"/>
+  <xr:revisionPtr revIDLastSave="301" documentId="11_CF4C787892D7E5F60EE01957CA2528E350C20E1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE04919C-2173-4858-A8CC-EBC40C32A362}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Página1!$B$2:$H$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Página1!$C$2:$I$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -77,11 +77,6 @@
     <t>Criação de um token para cada fazenda do usuário</t>
   </si>
   <si>
-    <t xml:space="preserve">Dificuldade de comunicação entre integrantes da
-equipe
-</t>
-  </si>
-  <si>
     <t>Problemas de conexão com a internet</t>
   </si>
   <si>
@@ -116,13 +111,74 @@
   </si>
   <si>
     <t xml:space="preserve">Fazendo as estimatívas dos tamanhos dos requisitos e criando o gráfico de Burndown </t>
+  </si>
+  <si>
+    <t>Atrasos nas entregas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balancear as sprints de modo que os pesos das entregas sejam compatíveis com a produção da nossa equipe </t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Dificuldade de comunicação entre integrantes da
+equipe</t>
+  </si>
+  <si>
+    <t>Alto (3)</t>
+  </si>
+  <si>
+    <t>Médio (2)</t>
+  </si>
+  <si>
+    <t>Baixo (1)</t>
+  </si>
+  <si>
+    <t>Pouco provável (1)</t>
+  </si>
+  <si>
+    <t>Provável (2)</t>
+  </si>
+  <si>
+    <t>Muito Provável (3)</t>
+  </si>
+  <si>
+    <t>Probabilidade</t>
+  </si>
+  <si>
+    <t>Impacto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -141,19 +197,41 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF63D297"/>
-        <bgColor rgb="FF63D297"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -163,18 +241,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7F9EF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor rgb="FFE7F9EF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FF63D297"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -292,37 +412,182 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -388,6 +653,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,24 +860,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -626,29 +896,31 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -656,31 +928,33 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="6">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="5">
         <v>3</v>
       </c>
-      <c r="F3" s="6">
-        <f t="shared" ref="F3:F9" si="0">PRODUCT(D3:E3)</f>
+      <c r="G3" s="5">
+        <f>PRODUCT(E3:F3)</f>
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="5"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -688,31 +962,33 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
-      <c r="B4" s="7">
+      <c r="B4" s="26">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="C4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="28">
         <v>1</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="28">
         <v>2</v>
       </c>
-      <c r="F4" s="7">
-        <f t="shared" si="0"/>
+      <c r="G4" s="28">
+        <f>PRODUCT(E4:F4)</f>
         <v>2</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="28" t="s">
+        <v>17</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -720,31 +996,33 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" s="6">
+      <c r="B5" s="14">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="6">
+      <c r="G5" s="6">
+        <f>PRODUCT(E5:F5)</f>
         <v>3</v>
       </c>
-      <c r="F5" s="8">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -752,31 +1030,33 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="7">
+      <c r="B6" s="26">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="28">
+        <v>1</v>
+      </c>
+      <c r="F6" s="28">
+        <v>2</v>
+      </c>
+      <c r="G6" s="28">
+        <f>PRODUCT(E6:F6)</f>
+        <v>2</v>
+      </c>
+      <c r="H6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7">
-        <v>2</v>
-      </c>
-      <c r="E6" s="7">
-        <v>3</v>
-      </c>
-      <c r="F6" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="28" t="s">
+        <v>19</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -784,31 +1064,33 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="6">
+      <c r="B7" s="14">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5">
+        <f>PRODUCT(E7:F7)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6">
-        <v>3</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="5"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -816,31 +1098,33 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="7">
+      <c r="B8" s="26">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="28">
+        <v>2</v>
+      </c>
+      <c r="F8" s="28">
+        <v>3</v>
+      </c>
+      <c r="G8" s="28">
+        <f>PRODUCT(E8:F8)</f>
+        <v>6</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -848,31 +1132,33 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="10">
+    <row r="9" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="14">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="8">
         <v>2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="F9" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="10">
-        <f t="shared" si="0"/>
+      <c r="G9" s="8">
+        <f>PRODUCT(E9:F9)</f>
         <v>6</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -880,18 +1166,33 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="11">
+    <row r="10" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="26">
         <v>8</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="5"/>
+      <c r="C10" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="32">
+        <v>2</v>
+      </c>
+      <c r="F10" s="32">
+        <v>3</v>
+      </c>
+      <c r="G10" s="33">
+        <f>PRODUCT(E10:F10)</f>
+        <v>6</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>21</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -899,37 +1200,27 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="5"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -941,14 +1232,10 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -961,10 +1248,10 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -975,16 +1262,11 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -995,16 +1277,11 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1014,16 +1291,11 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1033,13 +1305,8 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1053,19 +1320,13 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1079,7 +1340,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1099,7 +1360,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1119,7 +1380,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1138,7 +1399,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1157,7 +1418,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1175,7 +1436,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1193,7 +1454,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1211,15 +1472,17 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="E27" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1227,17 +1490,79 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
+    <row r="28" spans="1:18" ht="18" x14ac:dyDescent="0.2">
+      <c r="E28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="21">
+        <v>3</v>
+      </c>
+      <c r="G28" s="22">
+        <v>6</v>
+      </c>
+      <c r="H28" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="18" x14ac:dyDescent="0.2">
+      <c r="E29" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="23">
+        <v>2</v>
+      </c>
+      <c r="G29" s="21">
+        <v>4</v>
+      </c>
+      <c r="H29" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.2">
+      <c r="E30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="23">
+        <v>1</v>
+      </c>
+      <c r="G30" s="23">
+        <v>2</v>
+      </c>
+      <c r="H30" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.2">
+      <c r="E31" s="11"/>
+      <c r="F31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B2:H9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="F3:F9">
+  <autoFilter ref="C2:I9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="G3:G10">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>9</formula>
     </cfRule>
     <cfRule type="notContainsText" dxfId="4" priority="6" operator="notContains" text="1, 2, 3, 4, 6, 9">
-      <formula>ISERROR(SEARCH(("1, 2, 3, 4, 6, 9"),(F3)))</formula>
+      <formula>ISERROR(SEARCH(("1, 2, 3, 4, 6, 9"),(G3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F10">
+  <conditionalFormatting sqref="G3:G10">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
       <formula>1</formula>
       <formula>2</formula>
@@ -1250,11 +1575,12 @@
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="G5">
     <cfRule type="notContainsText" dxfId="0" priority="5" operator="notContains" text="1, 2, 3, 4, 6, 9">
-      <formula>ISERROR(SEARCH(("1, 2, 3, 4, 6, 9"),(F5)))</formula>
+      <formula>ISERROR(SEARCH(("1, 2, 3, 4, 6, 9"),(G5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>